<commit_message>
Updated project with WIP
</commit_message>
<xml_diff>
--- a/work-in-progress/translated_distinct.xlsx
+++ b/work-in-progress/translated_distinct.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/DKS02/runtime_environments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C53D1EC-D966-1742-ACB0-C4E299BCB5B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6CA93E2-83BD-4042-A6A7-18FA7A09C05B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="67200" windowHeight="36200" activeTab="6" xr2:uid="{8672D16A-3DAD-1242-8D32-39C1CA3ADB53}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="67200" windowHeight="36200" activeTab="7" xr2:uid="{8672D16A-3DAD-1242-8D32-39C1CA3ADB53}"/>
   </bookViews>
   <sheets>
     <sheet name="ALL-SDs" sheetId="1" r:id="rId1"/>
@@ -20,10 +20,10 @@
     <sheet name="Filtered-Unmapped" sheetId="4" r:id="rId5"/>
     <sheet name="latest" sheetId="6" r:id="rId6"/>
     <sheet name="unmapped-latest" sheetId="7" r:id="rId7"/>
-    <sheet name="Sheet3" sheetId="8" r:id="rId8"/>
+    <sheet name="Parser failures" sheetId="8" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="failed_1" localSheetId="7">Sheet3!$A$1:$A$114</definedName>
+    <definedName name="failed_1" localSheetId="7">'Parser failures'!$A$1:$A$114</definedName>
     <definedName name="translated_distinct_1" localSheetId="0">'ALL-SDs'!$A$2:$F$157</definedName>
     <definedName name="translated_distinct_1" localSheetId="3">FILTERED!$A$1:$F$110</definedName>
     <definedName name="translated_distinct_1" localSheetId="5">latest!$A$1:$F$168</definedName>
@@ -9455,7 +9455,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F73B0A3B-9AA2-AB40-A472-CE62ABC39DCA}">
   <dimension ref="A1:F168"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView topLeftCell="A21" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="22" x14ac:dyDescent="0.2"/>
   <cols>
@@ -12837,7 +12837,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AF39944-5B0C-5A44-ABE8-5B236B66BAB8}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
@@ -12946,7 +12946,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AE568AF-0E3F-2E4B-A260-DA46B07B0543}">
   <dimension ref="A1:A114"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="123.1640625" defaultRowHeight="21" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>